<commit_message>
Fixed mislabeled monobactams, spelling of meningitidis
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexgoodell/code/antibiogram/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/Desktop/OneDrive - UCB-O365/Misc/antibiogram.mine/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33640" windowHeight="20580" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t>Ceftriaxone</t>
-  </si>
-  <si>
-    <t>N. meningitis</t>
   </si>
   <si>
     <t>N. gonorrhoeae</t>
@@ -243,6 +237,15 @@
   </si>
   <si>
     <t>Streptococci</t>
+  </si>
+  <si>
+    <t>Carbapenems</t>
+  </si>
+  <si>
+    <t>Aztreonam</t>
+  </si>
+  <si>
+    <t>N. meningitidis</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +423,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE9C872"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,7 +587,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -623,85 +632,20 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -752,6 +696,9 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,6 +714,15 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,17 +741,79 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1091,13 +1109,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1126,7 @@
     <col min="8" max="8" width="14.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="2"/>
     <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="19.5" style="2" customWidth="1"/>
     <col min="13" max="13" width="16.5" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
@@ -1119,47 +1135,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="43" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="67"/>
+      <c r="L1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="45" t="s">
-        <v>22</v>
+      <c r="M1" s="24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="74" t="s">
-        <v>59</v>
+      <c r="D2" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>4</v>
@@ -1167,18 +1183,18 @@
       <c r="I2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="72" t="s">
+      <c r="J2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="46"/>
+      <c r="K2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="23"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1196,19 +1212,19 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="O3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="18" t="str">
+      <c r="C4" s="68" t="str">
         <f>O4</f>
         <v>Naficillin/Oxacillin</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1219,47 +1235,47 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="O4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="18" t="str">
+      <c r="D5" s="68" t="str">
         <f>O5</f>
         <v>Ampicillin/Amoxicillin</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="O5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="21" t="str">
+      <c r="C6" s="56" t="str">
         <f>O6</f>
         <v>Cefazolin, cephalexin</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="58"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1272,17 +1288,17 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="21" t="str">
+      <c r="C7" s="56" t="str">
         <f>O7</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="23"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="58"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1297,25 +1313,25 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>46</v>
+      <c r="A8" s="38" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="21" t="str">
+      <c r="C8" s="56" t="str">
         <f>O8</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="23"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="21" t="str">
+      <c r="I8" s="56" t="str">
         <f>O8</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="23"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="58"/>
       <c r="L8" s="4"/>
       <c r="M8" s="6"/>
       <c r="O8" s="2" t="s">
@@ -1323,443 +1339,458 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="21" t="str">
+      <c r="D9" s="56" t="str">
         <f>O9</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="23"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="6"/>
       <c r="O9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="33" t="str">
-        <f t="shared" ref="C10:C18" si="0">O10</f>
+      <c r="C10" s="59" t="str">
+        <f t="shared" ref="C10:C19" si="0">O10</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="23"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
       <c r="L10" s="4"/>
       <c r="M10" s="6"/>
       <c r="O10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>48</v>
+      <c r="A11" s="38" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="24" t="str">
+      <c r="C11" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Amoxicillin + clavulanate (Augmentin)</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M11" s="4"/>
       <c r="O11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="24" t="str">
+      <c r="C12" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Ampacillin + sulbactam (Unasyn)</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M12" s="4"/>
       <c r="O12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="35" t="str">
+      <c r="C13" s="61" t="str">
         <f t="shared" si="0"/>
         <v>Piperacillin + tazobactam (Zosyn)</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="62"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="35" t="str">
+      <c r="K13" s="61" t="str">
         <f>O13</f>
         <v>Piperacillin + tazobactam (Zosyn)</v>
       </c>
-      <c r="L13" s="36"/>
+      <c r="L13" s="62"/>
       <c r="M13" s="4"/>
       <c r="O13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>17</v>
+      <c r="A14" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="38" t="str">
+      <c r="C14" s="64" t="str">
         <f t="shared" si="0"/>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="66"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="38" t="str">
+      <c r="I14" s="64" t="str">
         <f>O14</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="66"/>
       <c r="M14" s="4"/>
       <c r="O14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="41" t="str">
+      <c r="C15" s="64" t="str">
         <f t="shared" si="0"/>
         <v>Imipenem, Meropenem</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="40"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66"/>
       <c r="M15" s="4"/>
       <c r="O15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="9" t="str">
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="4"/>
+      <c r="O16" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="59" t="str">
-        <f>O16</f>
+      <c r="D17" s="4"/>
+      <c r="E17" s="39" t="str">
+        <f>O17</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="O16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="59" t="str">
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="O17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Levofloxacin</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="9" t="str">
-        <f>O17</f>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="9" t="str">
+        <f>O18</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="29" t="str">
+      <c r="O18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="38"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="29" t="str">
-        <f>O18</f>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="44" t="str">
+        <f>O19</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="31"/>
-      <c r="O18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="66" t="str">
-        <f>O19</f>
-        <v>Gent/Tobra/Amikacin</v>
-      </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="46"/>
       <c r="O19" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="48" t="str">
+        <v>48</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="49" t="str">
         <f>O20</f>
-        <v>Clindamyacin</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+        <v>Gent/Tobra/Amikacin</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="15" t="str">
-        <f>O20</f>
-        <v>Clindamyacin</v>
-      </c>
-      <c r="M20" s="71"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
       <c r="O20" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="64" t="str">
+        <v>26</v>
+      </c>
+      <c r="B21" s="27" t="str">
         <f>O21</f>
-        <v>Azithromycin</v>
-      </c>
-      <c r="D21" s="65"/>
+        <v>Clindamyacin</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="10" t="str">
+      <c r="K21" s="6"/>
+      <c r="L21" s="15" t="str">
         <f>O21</f>
-        <v>Azithromycin</v>
-      </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="70" t="str">
-        <f>O21</f>
-        <v>Azithromycin</v>
-      </c>
+        <v>Clindamyacin</v>
+      </c>
+      <c r="M21" s="18"/>
       <c r="O21" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="51" t="str">
+      <c r="C22" s="47" t="str">
         <f>O22</f>
-        <v>Doxyclycine</v>
-      </c>
-      <c r="E22" s="52"/>
+        <v>Azithromycin</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="11" t="str">
+      <c r="K22" s="10" t="str">
         <f>O22</f>
-        <v>Doxyclycine</v>
+        <v>Azithromycin</v>
       </c>
       <c r="L22" s="6"/>
-      <c r="M22" s="11" t="str">
+      <c r="M22" s="17" t="str">
         <f>O22</f>
-        <v>Doxyclycine</v>
+        <v>Azithromycin</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="53" t="str">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="30" t="str">
         <f>O23</f>
-        <v>Vancomycin</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="6"/>
+        <v>Doxyclycine</v>
+      </c>
+      <c r="E23" s="31"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="K23" s="11" t="str">
+        <f>O23</f>
+        <v>Doxyclycine</v>
+      </c>
       <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="M23" s="11" t="str">
+        <f>O23</f>
+        <v>Doxyclycine</v>
+      </c>
       <c r="O23" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="56" t="str">
+        <v>49</v>
+      </c>
+      <c r="B24" s="32" t="str">
         <f>O24</f>
-        <v>TMP/SMX (Bactrim)</v>
-      </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="12" t="s">
-        <v>26</v>
-      </c>
+        <v>Vancomycin</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="4"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="O24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="35" t="str">
+        <f>O25</f>
+        <v>TMP/SMX (Bactrim)</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="6"/>
+      <c r="O25" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L25" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
+    </row>
+    <row r="27" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="C17:K17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="I18:M18"/>
+  <mergeCells count="36">
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I19:M19"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="I8:K8"/>
@@ -1770,17 +1801,25 @@
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="I14:L14"/>
     <mergeCell ref="C15:L15"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refreshed jpg, added pdf
</commit_message>
<xml_diff>
--- a/antibiogram.xlsx
+++ b/antibiogram.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/Desktop/OneDrive - UCB-O365/Misc/antibiogram.mine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexgoodell/code/antibiogram/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC60F5C9-5DD6-0346-A693-AA7C38F7B195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="25180" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$27</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -251,8 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,33 +289,43 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color theme="2" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -587,234 +598,235 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -838,6 +850,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1105,18 +1120,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7:G7"/>
+      <selection pane="topRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
@@ -1127,445 +1142,447 @@
     <col min="9" max="9" width="10.83203125" style="2"/>
     <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22" style="2" customWidth="1"/>
     <col min="13" max="13" width="16.5" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
     <col min="15" max="15" width="33.6640625" style="2" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="72" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="67" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="67"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="3"/>
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:15" ht="17">
+      <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="str">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="str">
         <f>O3</f>
         <v>Penicillin G</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
       <c r="O3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:15" ht="17">
+      <c r="A4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="68" t="str">
+      <c r="B4" s="16"/>
+      <c r="C4" s="18" t="str">
         <f>O4</f>
         <v>Naficillin/Oxacillin</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:15" ht="17">
+      <c r="A5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="68" t="str">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="18" t="str">
         <f>O5</f>
         <v>Ampicillin/Amoxicillin</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
       <c r="O5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:15" ht="17">
+      <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="56" t="str">
+      <c r="B6" s="16"/>
+      <c r="C6" s="21" t="str">
         <f>O6</f>
         <v>Cefazolin, cephalexin</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="24"/>
       <c r="O6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:15" ht="17">
+      <c r="A7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="56" t="str">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="str">
         <f>O7</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="7" t="str">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="26" t="str">
         <f>O7</f>
         <v>Cephotetan, Cefoxitin</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="24"/>
       <c r="O7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:15">
+      <c r="A8" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="56" t="str">
+      <c r="B8" s="16"/>
+      <c r="C8" s="21" t="str">
         <f>O8</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="56" t="str">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="21" t="str">
         <f>O8</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="57"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="24"/>
       <c r="O8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="56" t="str">
+    <row r="9" spans="1:15">
+      <c r="A9" s="27"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="21" t="str">
         <f>O9</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="24"/>
       <c r="O9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:15" ht="17">
+      <c r="A10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="59" t="str">
+      <c r="B10" s="16"/>
+      <c r="C10" s="28" t="str">
         <f t="shared" ref="C10:C19" si="0">O10</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="24"/>
       <c r="O10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:15">
+      <c r="A11" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="53" t="str">
+      <c r="B11" s="16"/>
+      <c r="C11" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Amoxicillin + clavulanate (Augmentin)</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="8" t="s">
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="16"/>
       <c r="O11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="53" t="str">
+    <row r="12" spans="1:15">
+      <c r="A12" s="27"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Ampacillin + sulbactam (Unasyn)</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="8" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="16"/>
       <c r="O12" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="61" t="str">
+    <row r="13" spans="1:15">
+      <c r="A13" s="27"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Piperacillin + tazobactam (Zosyn)</v>
       </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="61" t="str">
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="34" t="str">
         <f>O13</f>
         <v>Piperacillin + tazobactam (Zosyn)</v>
       </c>
-      <c r="L13" s="62"/>
-      <c r="M13" s="4"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="16"/>
       <c r="O13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
+    <row r="14" spans="1:15">
+      <c r="A14" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="64" t="str">
+      <c r="B14" s="16"/>
+      <c r="C14" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="64" t="str">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="37" t="str">
         <f>O14</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="4"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="16"/>
       <c r="O14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="64" t="str">
+    <row r="15" spans="1:15">
+      <c r="A15" s="27"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Imipenem, Meropenem</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="4"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="16"/>
       <c r="O15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:15" ht="17">
+      <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="77"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="4"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="16"/>
       <c r="O16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="38" t="s">
+    <row r="17" spans="1:15">
+      <c r="A17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="9" t="str">
+      <c r="B17" s="16"/>
+      <c r="C17" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="39" t="str">
+      <c r="D17" s="16"/>
+      <c r="E17" s="45" t="str">
         <f>O17</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
       <c r="O17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="39" t="str">
+    <row r="18" spans="1:15">
+      <c r="A18" s="27"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="9" t="str">
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="44" t="str">
         <f>O18</f>
         <v>Levofloxacin</v>
       </c>
@@ -1573,101 +1590,101 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="44" t="str">
+    <row r="19" spans="1:15">
+      <c r="A19" s="27"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="44" t="str">
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="50" t="str">
         <f>O19</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="46"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="52"/>
       <c r="O19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:15" ht="17">
+      <c r="A20" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="49" t="str">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="53" t="str">
         <f>O20</f>
         <v>Gent/Tobra/Amikacin</v>
       </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
       <c r="O20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:15" ht="17">
+      <c r="A21" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="27" t="str">
+      <c r="B21" s="57" t="str">
         <f>O21</f>
         <v>Clindamyacin</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="15" t="str">
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="60" t="str">
         <f>O21</f>
         <v>Clindamyacin</v>
       </c>
-      <c r="M21" s="18"/>
+      <c r="M21" s="61"/>
       <c r="O21" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:15" ht="17">
+      <c r="A22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="47" t="str">
+      <c r="B22" s="24"/>
+      <c r="C22" s="62" t="str">
         <f>O22</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="10" t="str">
+      <c r="D22" s="63"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="64" t="str">
         <f>O22</f>
         <v>Azithromycin</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="17" t="str">
+      <c r="L22" s="24"/>
+      <c r="M22" s="65" t="str">
         <f>O22</f>
         <v>Azithromycin</v>
       </c>
@@ -1675,28 +1692,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:15" ht="17">
+      <c r="A23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="30" t="str">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="66" t="str">
         <f>O23</f>
         <v>Doxyclycine</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="11" t="str">
+      <c r="E23" s="67"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="68" t="str">
         <f>O23</f>
         <v>Doxyclycine</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="11" t="str">
+      <c r="L23" s="24"/>
+      <c r="M23" s="68" t="str">
         <f>O23</f>
         <v>Doxyclycine</v>
       </c>
@@ -1704,83 +1721,114 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:15" ht="17">
+      <c r="A24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="32" t="str">
+      <c r="B24" s="69" t="str">
         <f>O24</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
       <c r="O24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:15" ht="17">
+      <c r="A25" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="35" t="str">
+      <c r="B25" s="72" t="str">
         <f>O25</f>
         <v>TMP/SMX (Bactrim)</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="12" t="s">
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="12" t="s">
+      <c r="J25" s="24"/>
+      <c r="K25" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="24"/>
       <c r="O25" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:15" ht="17">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L26" s="13" t="s">
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="77" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+      <c r="M26" s="76"/>
+    </row>
+    <row r="27" spans="1:15" ht="36" customHeight="1">
+      <c r="A27" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -1797,29 +1845,9 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>